<commit_message>
DMB07 - modified bill filling and created unit tests project
</commit_message>
<xml_diff>
--- a/DoMyBilling/DoMyBilling/ExcelBills/BillTemplate.xlsx
+++ b/DoMyBilling/DoMyBilling/ExcelBills/BillTemplate.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Kaposvári Márk\source\repos\IRF_Project\DoMyBilling\DoMyBilling\ExcelBills\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E6685EB6-FE9A-4227-B7C4-75C5C2D44B74}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5D50220D-D823-4F8D-8ACA-685DDED6F481}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{F2786273-DC1B-47B2-AC3A-962882F38129}"/>
   </bookViews>
@@ -275,7 +275,7 @@
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="25">
+  <cellXfs count="26">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
@@ -294,12 +294,6 @@
     <xf numFmtId="0" fontId="0" fillId="3" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
@@ -323,6 +317,15 @@
     </xf>
     <xf numFmtId="49" fontId="0" fillId="2" borderId="4" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="49" fontId="0" fillId="2" borderId="11" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normál" xfId="0" builtinId="0"/>
@@ -638,10 +641,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6DEC2F63-A0AF-4687-BE6D-74EE77351709}">
-  <dimension ref="B1:E10"/>
+  <dimension ref="A1:H47"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D10" sqref="D10"/>
+      <selection activeCell="G4" sqref="G4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -653,41 +656,58 @@
     <col min="6" max="6" width="9.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B1" s="17" t="s">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A1" s="1"/>
+      <c r="B1" s="15" t="s">
         <v>5</v>
       </c>
-      <c r="C1" s="18"/>
-      <c r="D1" s="18"/>
-      <c r="E1" s="19"/>
-    </row>
-    <row r="2" spans="2:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B2" s="20"/>
-      <c r="C2" s="21"/>
-      <c r="D2" s="21"/>
-      <c r="E2" s="22"/>
-    </row>
-    <row r="3" spans="2:5" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B3" s="12" t="s">
+      <c r="C1" s="16"/>
+      <c r="D1" s="16"/>
+      <c r="E1" s="17"/>
+      <c r="F1" s="1"/>
+      <c r="G1" s="1"/>
+      <c r="H1" s="1"/>
+    </row>
+    <row r="2" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A2" s="1"/>
+      <c r="B2" s="18"/>
+      <c r="C2" s="19"/>
+      <c r="D2" s="19"/>
+      <c r="E2" s="20"/>
+      <c r="F2" s="1"/>
+      <c r="G2" s="1"/>
+      <c r="H2" s="1"/>
+    </row>
+    <row r="3" spans="1:8" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A3" s="1"/>
+      <c r="B3" s="23" t="s">
         <v>12</v>
       </c>
-      <c r="C3" s="13"/>
-      <c r="D3" s="13" t="s">
+      <c r="C3" s="24"/>
+      <c r="D3" s="24" t="s">
         <v>11</v>
       </c>
-      <c r="E3" s="13"/>
-    </row>
-    <row r="4" spans="2:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B4" s="14" t="s">
+      <c r="E3" s="25"/>
+      <c r="F3" s="1"/>
+      <c r="G3" s="1"/>
+      <c r="H3" s="1"/>
+    </row>
+    <row r="4" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A4" s="1"/>
+      <c r="B4" s="12" t="s">
         <v>1</v>
       </c>
-      <c r="C4" s="15"/>
-      <c r="D4" s="15" t="s">
+      <c r="C4" s="13"/>
+      <c r="D4" s="13" t="s">
         <v>3</v>
       </c>
-      <c r="E4" s="16"/>
-    </row>
-    <row r="5" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="E4" s="14"/>
+      <c r="F4" s="1"/>
+      <c r="G4" s="1"/>
+      <c r="H4" s="1"/>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A5" s="1"/>
       <c r="B5" s="3" t="s">
         <v>2</v>
       </c>
@@ -696,8 +716,12 @@
         <v>4</v>
       </c>
       <c r="E5" s="5"/>
-    </row>
-    <row r="6" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="F5" s="1"/>
+      <c r="G5" s="1"/>
+      <c r="H5" s="1"/>
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A6" s="1"/>
       <c r="B6" s="6" t="s">
         <v>8</v>
       </c>
@@ -706,8 +730,12 @@
         <v>8</v>
       </c>
       <c r="E6" s="7"/>
-    </row>
-    <row r="7" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="F6" s="1"/>
+      <c r="G6" s="1"/>
+      <c r="H6" s="1"/>
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A7" s="1"/>
       <c r="B7" s="6" t="s">
         <v>9</v>
       </c>
@@ -716,24 +744,36 @@
         <v>9</v>
       </c>
       <c r="E7" s="7"/>
-    </row>
-    <row r="8" spans="2:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="F7" s="1"/>
+      <c r="G7" s="1"/>
+      <c r="H7" s="1"/>
+    </row>
+    <row r="8" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A8" s="1"/>
       <c r="B8" s="8" t="s">
         <v>0</v>
       </c>
-      <c r="C8" s="23"/>
+      <c r="C8" s="21"/>
       <c r="D8" s="8" t="s">
         <v>0</v>
       </c>
-      <c r="E8" s="24"/>
-    </row>
-    <row r="9" spans="2:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="E8" s="22"/>
+      <c r="F8" s="1"/>
+      <c r="G8" s="1"/>
+      <c r="H8" s="1"/>
+    </row>
+    <row r="9" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A9" s="1"/>
       <c r="B9" s="1"/>
       <c r="C9" s="1"/>
       <c r="D9" s="1"/>
       <c r="E9" s="1"/>
-    </row>
-    <row r="10" spans="2:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="F9" s="1"/>
+      <c r="G9" s="1"/>
+      <c r="H9" s="1"/>
+    </row>
+    <row r="10" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A10" s="1"/>
       <c r="B10" s="9" t="s">
         <v>6</v>
       </c>
@@ -746,6 +786,379 @@
       <c r="E10" s="11" t="s">
         <v>10</v>
       </c>
+      <c r="F10" s="1"/>
+      <c r="G10" s="1"/>
+      <c r="H10" s="1"/>
+    </row>
+    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A11" s="1"/>
+      <c r="B11" s="1"/>
+      <c r="C11" s="1"/>
+      <c r="D11" s="1"/>
+      <c r="E11" s="1"/>
+      <c r="F11" s="1"/>
+      <c r="G11" s="1"/>
+      <c r="H11" s="1"/>
+    </row>
+    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A12" s="1"/>
+      <c r="B12" s="1"/>
+      <c r="C12" s="1"/>
+      <c r="D12" s="1"/>
+      <c r="E12" s="1"/>
+      <c r="F12" s="1"/>
+      <c r="G12" s="1"/>
+      <c r="H12" s="1"/>
+    </row>
+    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A13" s="1"/>
+      <c r="B13" s="1"/>
+      <c r="C13" s="1"/>
+      <c r="D13" s="1"/>
+      <c r="E13" s="1"/>
+      <c r="F13" s="1"/>
+      <c r="G13" s="1"/>
+      <c r="H13" s="1"/>
+    </row>
+    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A14" s="1"/>
+      <c r="B14" s="1"/>
+      <c r="C14" s="1"/>
+      <c r="D14" s="1"/>
+      <c r="E14" s="1"/>
+      <c r="F14" s="1"/>
+      <c r="G14" s="1"/>
+      <c r="H14" s="1"/>
+    </row>
+    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A15" s="1"/>
+      <c r="B15" s="1"/>
+      <c r="C15" s="1"/>
+      <c r="D15" s="1"/>
+      <c r="E15" s="1"/>
+      <c r="F15" s="1"/>
+      <c r="G15" s="1"/>
+      <c r="H15" s="1"/>
+    </row>
+    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A16" s="1"/>
+      <c r="B16" s="1"/>
+      <c r="C16" s="1"/>
+      <c r="D16" s="1"/>
+      <c r="E16" s="1"/>
+      <c r="F16" s="1"/>
+      <c r="G16" s="1"/>
+      <c r="H16" s="1"/>
+    </row>
+    <row r="17" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A17" s="1"/>
+      <c r="B17" s="1"/>
+      <c r="C17" s="1"/>
+      <c r="D17" s="1"/>
+      <c r="E17" s="1"/>
+      <c r="F17" s="1"/>
+      <c r="G17" s="1"/>
+      <c r="H17" s="1"/>
+    </row>
+    <row r="18" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A18" s="1"/>
+      <c r="B18" s="1"/>
+      <c r="C18" s="1"/>
+      <c r="D18" s="1"/>
+      <c r="E18" s="1"/>
+      <c r="F18" s="1"/>
+      <c r="G18" s="1"/>
+      <c r="H18" s="1"/>
+    </row>
+    <row r="19" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A19" s="1"/>
+      <c r="B19" s="1"/>
+      <c r="C19" s="1"/>
+      <c r="D19" s="1"/>
+      <c r="E19" s="1"/>
+      <c r="F19" s="1"/>
+      <c r="G19" s="1"/>
+      <c r="H19" s="1"/>
+    </row>
+    <row r="20" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A20" s="1"/>
+      <c r="B20" s="1"/>
+      <c r="C20" s="1"/>
+      <c r="D20" s="1"/>
+      <c r="E20" s="1"/>
+      <c r="F20" s="1"/>
+      <c r="G20" s="1"/>
+      <c r="H20" s="1"/>
+    </row>
+    <row r="21" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A21" s="1"/>
+      <c r="B21" s="1"/>
+      <c r="C21" s="1"/>
+      <c r="D21" s="1"/>
+      <c r="E21" s="1"/>
+      <c r="F21" s="1"/>
+      <c r="G21" s="1"/>
+      <c r="H21" s="1"/>
+    </row>
+    <row r="22" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A22" s="1"/>
+      <c r="B22" s="1"/>
+      <c r="C22" s="1"/>
+      <c r="D22" s="1"/>
+      <c r="E22" s="1"/>
+      <c r="F22" s="1"/>
+      <c r="G22" s="1"/>
+      <c r="H22" s="1"/>
+    </row>
+    <row r="23" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A23" s="1"/>
+      <c r="B23" s="1"/>
+      <c r="C23" s="1"/>
+      <c r="D23" s="1"/>
+      <c r="E23" s="1"/>
+      <c r="F23" s="1"/>
+      <c r="G23" s="1"/>
+      <c r="H23" s="1"/>
+    </row>
+    <row r="24" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A24" s="1"/>
+      <c r="B24" s="1"/>
+      <c r="C24" s="1"/>
+      <c r="D24" s="1"/>
+      <c r="E24" s="1"/>
+      <c r="F24" s="1"/>
+      <c r="G24" s="1"/>
+      <c r="H24" s="1"/>
+    </row>
+    <row r="25" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A25" s="1"/>
+      <c r="B25" s="1"/>
+      <c r="C25" s="1"/>
+      <c r="D25" s="1"/>
+      <c r="E25" s="1"/>
+      <c r="F25" s="1"/>
+      <c r="G25" s="1"/>
+      <c r="H25" s="1"/>
+    </row>
+    <row r="26" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A26" s="1"/>
+      <c r="B26" s="1"/>
+      <c r="C26" s="1"/>
+      <c r="D26" s="1"/>
+      <c r="E26" s="1"/>
+      <c r="F26" s="1"/>
+      <c r="G26" s="1"/>
+      <c r="H26" s="1"/>
+    </row>
+    <row r="27" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A27" s="1"/>
+      <c r="B27" s="1"/>
+      <c r="C27" s="1"/>
+      <c r="D27" s="1"/>
+      <c r="E27" s="1"/>
+      <c r="F27" s="1"/>
+      <c r="G27" s="1"/>
+      <c r="H27" s="1"/>
+    </row>
+    <row r="28" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A28" s="1"/>
+      <c r="B28" s="1"/>
+      <c r="C28" s="1"/>
+      <c r="D28" s="1"/>
+      <c r="E28" s="1"/>
+      <c r="F28" s="1"/>
+      <c r="G28" s="1"/>
+      <c r="H28" s="1"/>
+    </row>
+    <row r="29" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A29" s="1"/>
+      <c r="B29" s="1"/>
+      <c r="C29" s="1"/>
+      <c r="D29" s="1"/>
+      <c r="E29" s="1"/>
+      <c r="F29" s="1"/>
+      <c r="G29" s="1"/>
+      <c r="H29" s="1"/>
+    </row>
+    <row r="30" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A30" s="1"/>
+      <c r="B30" s="1"/>
+      <c r="C30" s="1"/>
+      <c r="D30" s="1"/>
+      <c r="E30" s="1"/>
+      <c r="F30" s="1"/>
+      <c r="G30" s="1"/>
+      <c r="H30" s="1"/>
+    </row>
+    <row r="31" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A31" s="1"/>
+      <c r="B31" s="1"/>
+      <c r="C31" s="1"/>
+      <c r="D31" s="1"/>
+      <c r="E31" s="1"/>
+      <c r="F31" s="1"/>
+      <c r="G31" s="1"/>
+      <c r="H31" s="1"/>
+    </row>
+    <row r="32" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A32" s="1"/>
+      <c r="B32" s="1"/>
+      <c r="C32" s="1"/>
+      <c r="D32" s="1"/>
+      <c r="E32" s="1"/>
+      <c r="F32" s="1"/>
+      <c r="G32" s="1"/>
+      <c r="H32" s="1"/>
+    </row>
+    <row r="33" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A33" s="1"/>
+      <c r="B33" s="1"/>
+      <c r="C33" s="1"/>
+      <c r="D33" s="1"/>
+      <c r="E33" s="1"/>
+      <c r="F33" s="1"/>
+      <c r="G33" s="1"/>
+      <c r="H33" s="1"/>
+    </row>
+    <row r="34" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A34" s="1"/>
+      <c r="B34" s="1"/>
+      <c r="C34" s="1"/>
+      <c r="D34" s="1"/>
+      <c r="E34" s="1"/>
+      <c r="F34" s="1"/>
+      <c r="G34" s="1"/>
+      <c r="H34" s="1"/>
+    </row>
+    <row r="35" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A35" s="1"/>
+      <c r="B35" s="1"/>
+      <c r="C35" s="1"/>
+      <c r="D35" s="1"/>
+      <c r="E35" s="1"/>
+      <c r="F35" s="1"/>
+      <c r="G35" s="1"/>
+      <c r="H35" s="1"/>
+    </row>
+    <row r="36" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A36" s="1"/>
+      <c r="B36" s="1"/>
+      <c r="C36" s="1"/>
+      <c r="D36" s="1"/>
+      <c r="E36" s="1"/>
+      <c r="F36" s="1"/>
+      <c r="G36" s="1"/>
+      <c r="H36" s="1"/>
+    </row>
+    <row r="37" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A37" s="1"/>
+      <c r="B37" s="1"/>
+      <c r="C37" s="1"/>
+      <c r="D37" s="1"/>
+      <c r="E37" s="1"/>
+      <c r="F37" s="1"/>
+      <c r="G37" s="1"/>
+      <c r="H37" s="1"/>
+    </row>
+    <row r="38" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A38" s="1"/>
+      <c r="B38" s="1"/>
+      <c r="C38" s="1"/>
+      <c r="D38" s="1"/>
+      <c r="E38" s="1"/>
+      <c r="F38" s="1"/>
+      <c r="G38" s="1"/>
+      <c r="H38" s="1"/>
+    </row>
+    <row r="39" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A39" s="1"/>
+      <c r="B39" s="1"/>
+      <c r="C39" s="1"/>
+      <c r="D39" s="1"/>
+      <c r="E39" s="1"/>
+      <c r="F39" s="1"/>
+      <c r="G39" s="1"/>
+      <c r="H39" s="1"/>
+    </row>
+    <row r="40" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A40" s="1"/>
+      <c r="B40" s="1"/>
+      <c r="C40" s="1"/>
+      <c r="D40" s="1"/>
+      <c r="E40" s="1"/>
+      <c r="F40" s="1"/>
+      <c r="G40" s="1"/>
+      <c r="H40" s="1"/>
+    </row>
+    <row r="41" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A41" s="1"/>
+      <c r="B41" s="1"/>
+      <c r="C41" s="1"/>
+      <c r="D41" s="1"/>
+      <c r="E41" s="1"/>
+      <c r="F41" s="1"/>
+      <c r="G41" s="1"/>
+      <c r="H41" s="1"/>
+    </row>
+    <row r="42" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A42" s="1"/>
+      <c r="B42" s="1"/>
+      <c r="C42" s="1"/>
+      <c r="D42" s="1"/>
+      <c r="E42" s="1"/>
+      <c r="F42" s="1"/>
+      <c r="G42" s="1"/>
+      <c r="H42" s="1"/>
+    </row>
+    <row r="43" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A43" s="1"/>
+      <c r="B43" s="1"/>
+      <c r="C43" s="1"/>
+      <c r="D43" s="1"/>
+      <c r="E43" s="1"/>
+      <c r="F43" s="1"/>
+      <c r="G43" s="1"/>
+      <c r="H43" s="1"/>
+    </row>
+    <row r="44" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A44" s="1"/>
+      <c r="B44" s="1"/>
+      <c r="C44" s="1"/>
+      <c r="D44" s="1"/>
+      <c r="E44" s="1"/>
+      <c r="F44" s="1"/>
+      <c r="G44" s="1"/>
+      <c r="H44" s="1"/>
+    </row>
+    <row r="45" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A45" s="1"/>
+      <c r="B45" s="1"/>
+      <c r="C45" s="1"/>
+      <c r="D45" s="1"/>
+      <c r="E45" s="1"/>
+      <c r="F45" s="1"/>
+      <c r="G45" s="1"/>
+      <c r="H45" s="1"/>
+    </row>
+    <row r="46" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A46" s="1"/>
+      <c r="B46" s="1"/>
+      <c r="C46" s="1"/>
+      <c r="D46" s="1"/>
+      <c r="E46" s="1"/>
+      <c r="F46" s="1"/>
+      <c r="G46" s="1"/>
+      <c r="H46" s="1"/>
+    </row>
+    <row r="47" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A47" s="1"/>
+      <c r="B47" s="1"/>
+      <c r="C47" s="1"/>
+      <c r="D47" s="1"/>
+      <c r="E47" s="1"/>
+      <c r="F47" s="1"/>
+      <c r="G47" s="1"/>
+      <c r="H47" s="1"/>
     </row>
   </sheetData>
   <mergeCells count="1">

</xml_diff>

<commit_message>
DMB08 - added id generator and vat calculator, changed the template, also made textfields to be able to change the excel generation
</commit_message>
<xml_diff>
--- a/DoMyBilling/DoMyBilling/ExcelBills/BillTemplate.xlsx
+++ b/DoMyBilling/DoMyBilling/ExcelBills/BillTemplate.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Kaposvári Márk\source\repos\IRF_Project\DoMyBilling\DoMyBilling\ExcelBills\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5D50220D-D823-4F8D-8ACA-685DDED6F481}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F025A0A0-A5A4-4BBE-80DB-FC09C0DB29E8}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{F2786273-DC1B-47B2-AC3A-962882F38129}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{F2786273-DC1B-47B2-AC3A-962882F38129}"/>
   </bookViews>
   <sheets>
     <sheet name="Munka1" sheetId="1" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="16">
   <si>
     <t>Adószám:</t>
   </si>
@@ -59,6 +59,9 @@
     <t>Mennyiség</t>
   </si>
   <si>
+    <t>Nettó egységár</t>
+  </si>
+  <si>
     <t>Irányítószám, település:</t>
   </si>
   <si>
@@ -74,7 +77,10 @@
     <t>SzámlaID:</t>
   </si>
   <si>
-    <t>Egységár</t>
+    <t>Áfa</t>
+  </si>
+  <si>
+    <t>Áfa értéke</t>
   </si>
 </sst>
 </file>
@@ -275,15 +281,11 @@
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="26">
+  <cellXfs count="29">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="5" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="6" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="7" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="8" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="9" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="10" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -315,10 +317,35 @@
     <xf numFmtId="0" fontId="2" fillId="3" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="49" fontId="0" fillId="2" borderId="4" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="49" fontId="0" fillId="2" borderId="11" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="2" borderId="4" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="2" borderId="11" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -641,128 +668,146 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6DEC2F63-A0AF-4687-BE6D-74EE77351709}">
-  <dimension ref="A1:H47"/>
+  <dimension ref="A1:J47"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G4" sqref="G4"/>
+      <selection activeCell="E11" sqref="E11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="2" max="2" width="22" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="25.7109375" customWidth="1"/>
-    <col min="4" max="4" width="22" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="18.42578125" customWidth="1"/>
-    <col min="6" max="6" width="9.140625" customWidth="1"/>
+    <col min="3" max="3" width="16.42578125" customWidth="1"/>
+    <col min="4" max="4" width="21" customWidth="1"/>
+    <col min="5" max="5" width="23.140625" customWidth="1"/>
+    <col min="6" max="6" width="22" customWidth="1"/>
+    <col min="7" max="7" width="18.42578125" customWidth="1"/>
+    <col min="8" max="8" width="9.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A1" s="1"/>
-      <c r="B1" s="15" t="s">
+      <c r="B1" s="11" t="s">
         <v>5</v>
       </c>
-      <c r="C1" s="16"/>
-      <c r="D1" s="16"/>
-      <c r="E1" s="17"/>
-      <c r="F1" s="1"/>
-      <c r="G1" s="1"/>
+      <c r="C1" s="12"/>
+      <c r="D1" s="12"/>
+      <c r="E1" s="12"/>
+      <c r="F1" s="12"/>
+      <c r="G1" s="13"/>
       <c r="H1" s="1"/>
-    </row>
-    <row r="2" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="I1" s="1"/>
+      <c r="J1" s="1"/>
+    </row>
+    <row r="2" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A2" s="1"/>
-      <c r="B2" s="18"/>
-      <c r="C2" s="19"/>
-      <c r="D2" s="19"/>
-      <c r="E2" s="20"/>
-      <c r="F2" s="1"/>
-      <c r="G2" s="1"/>
+      <c r="B2" s="14"/>
+      <c r="C2" s="15"/>
+      <c r="D2" s="15"/>
+      <c r="E2" s="15"/>
+      <c r="F2" s="15"/>
+      <c r="G2" s="16"/>
       <c r="H2" s="1"/>
-    </row>
-    <row r="3" spans="1:8" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="I2" s="1"/>
+      <c r="J2" s="1"/>
+    </row>
+    <row r="3" spans="1:10" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A3" s="1"/>
-      <c r="B3" s="23" t="s">
+      <c r="B3" s="17" t="s">
+        <v>13</v>
+      </c>
+      <c r="C3" s="27"/>
+      <c r="D3" s="27"/>
+      <c r="E3" s="18" t="s">
         <v>12</v>
       </c>
-      <c r="C3" s="24"/>
-      <c r="D3" s="24" t="s">
-        <v>11</v>
-      </c>
-      <c r="E3" s="25"/>
-      <c r="F3" s="1"/>
-      <c r="G3" s="1"/>
+      <c r="F3" s="27"/>
+      <c r="G3" s="28"/>
       <c r="H3" s="1"/>
-    </row>
-    <row r="4" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="I3" s="1"/>
+      <c r="J3" s="1"/>
+    </row>
+    <row r="4" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A4" s="1"/>
-      <c r="B4" s="12" t="s">
+      <c r="B4" s="8" t="s">
         <v>1</v>
       </c>
-      <c r="C4" s="13"/>
-      <c r="D4" s="13" t="s">
+      <c r="C4" s="9"/>
+      <c r="D4" s="9"/>
+      <c r="E4" s="9" t="s">
         <v>3</v>
       </c>
-      <c r="E4" s="14"/>
-      <c r="F4" s="1"/>
-      <c r="G4" s="1"/>
+      <c r="F4" s="9"/>
+      <c r="G4" s="10"/>
       <c r="H4" s="1"/>
-    </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I4" s="1"/>
+      <c r="J4" s="1"/>
+    </row>
+    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A5" s="1"/>
-      <c r="B5" s="3" t="s">
+      <c r="B5" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="C5" s="4"/>
-      <c r="D5" s="3" t="s">
+      <c r="C5" s="19"/>
+      <c r="D5" s="20"/>
+      <c r="E5" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="E5" s="5"/>
-      <c r="F5" s="1"/>
-      <c r="G5" s="1"/>
+      <c r="F5" s="19"/>
+      <c r="G5" s="20"/>
       <c r="H5" s="1"/>
-    </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I5" s="1"/>
+      <c r="J5" s="1"/>
+    </row>
+    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A6" s="1"/>
-      <c r="B6" s="6" t="s">
-        <v>8</v>
-      </c>
-      <c r="C6" s="2"/>
-      <c r="D6" s="6" t="s">
-        <v>8</v>
-      </c>
-      <c r="E6" s="7"/>
-      <c r="F6" s="1"/>
-      <c r="G6" s="1"/>
+      <c r="B6" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="C6" s="21"/>
+      <c r="D6" s="22"/>
+      <c r="E6" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="F6" s="21"/>
+      <c r="G6" s="22"/>
       <c r="H6" s="1"/>
-    </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I6" s="1"/>
+      <c r="J6" s="1"/>
+    </row>
+    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A7" s="1"/>
-      <c r="B7" s="6" t="s">
-        <v>9</v>
-      </c>
-      <c r="C7" s="2"/>
-      <c r="D7" s="6" t="s">
-        <v>9</v>
-      </c>
-      <c r="E7" s="7"/>
-      <c r="F7" s="1"/>
-      <c r="G7" s="1"/>
+      <c r="B7" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="C7" s="21"/>
+      <c r="D7" s="22"/>
+      <c r="E7" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="F7" s="21"/>
+      <c r="G7" s="22"/>
       <c r="H7" s="1"/>
-    </row>
-    <row r="8" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="I7" s="1"/>
+      <c r="J7" s="1"/>
+    </row>
+    <row r="8" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A8" s="1"/>
-      <c r="B8" s="8" t="s">
+      <c r="B8" s="4" t="s">
         <v>0</v>
       </c>
-      <c r="C8" s="21"/>
-      <c r="D8" s="8" t="s">
+      <c r="C8" s="23"/>
+      <c r="D8" s="24"/>
+      <c r="E8" s="4" t="s">
         <v>0</v>
       </c>
-      <c r="E8" s="22"/>
-      <c r="F8" s="1"/>
-      <c r="G8" s="1"/>
+      <c r="F8" s="25"/>
+      <c r="G8" s="26"/>
       <c r="H8" s="1"/>
-    </row>
-    <row r="9" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="I8" s="1"/>
+      <c r="J8" s="1"/>
+    </row>
+    <row r="9" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A9" s="1"/>
       <c r="B9" s="1"/>
       <c r="C9" s="1"/>
@@ -771,26 +816,34 @@
       <c r="F9" s="1"/>
       <c r="G9" s="1"/>
       <c r="H9" s="1"/>
-    </row>
-    <row r="10" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="I9" s="1"/>
+      <c r="J9" s="1"/>
+    </row>
+    <row r="10" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A10" s="1"/>
-      <c r="B10" s="9" t="s">
+      <c r="B10" s="5" t="s">
         <v>6</v>
       </c>
-      <c r="C10" s="10" t="s">
+      <c r="C10" s="6" t="s">
         <v>7</v>
       </c>
-      <c r="D10" s="10" t="s">
-        <v>13</v>
-      </c>
-      <c r="E10" s="11" t="s">
-        <v>10</v>
-      </c>
-      <c r="F10" s="1"/>
-      <c r="G10" s="1"/>
+      <c r="D10" s="6" t="s">
+        <v>8</v>
+      </c>
+      <c r="E10" s="6" t="s">
+        <v>14</v>
+      </c>
+      <c r="F10" s="6" t="s">
+        <v>15</v>
+      </c>
+      <c r="G10" s="7" t="s">
+        <v>11</v>
+      </c>
       <c r="H10" s="1"/>
-    </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I10" s="1"/>
+      <c r="J10" s="1"/>
+    </row>
+    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A11" s="1"/>
       <c r="B11" s="1"/>
       <c r="C11" s="1"/>
@@ -799,8 +852,10 @@
       <c r="F11" s="1"/>
       <c r="G11" s="1"/>
       <c r="H11" s="1"/>
-    </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I11" s="1"/>
+      <c r="J11" s="1"/>
+    </row>
+    <row r="12" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A12" s="1"/>
       <c r="B12" s="1"/>
       <c r="C12" s="1"/>
@@ -809,8 +864,10 @@
       <c r="F12" s="1"/>
       <c r="G12" s="1"/>
       <c r="H12" s="1"/>
-    </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I12" s="1"/>
+      <c r="J12" s="1"/>
+    </row>
+    <row r="13" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A13" s="1"/>
       <c r="B13" s="1"/>
       <c r="C13" s="1"/>
@@ -819,8 +876,10 @@
       <c r="F13" s="1"/>
       <c r="G13" s="1"/>
       <c r="H13" s="1"/>
-    </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I13" s="1"/>
+      <c r="J13" s="1"/>
+    </row>
+    <row r="14" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A14" s="1"/>
       <c r="B14" s="1"/>
       <c r="C14" s="1"/>
@@ -829,8 +888,10 @@
       <c r="F14" s="1"/>
       <c r="G14" s="1"/>
       <c r="H14" s="1"/>
-    </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I14" s="1"/>
+      <c r="J14" s="1"/>
+    </row>
+    <row r="15" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A15" s="1"/>
       <c r="B15" s="1"/>
       <c r="C15" s="1"/>
@@ -839,8 +900,10 @@
       <c r="F15" s="1"/>
       <c r="G15" s="1"/>
       <c r="H15" s="1"/>
-    </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I15" s="1"/>
+      <c r="J15" s="1"/>
+    </row>
+    <row r="16" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A16" s="1"/>
       <c r="B16" s="1"/>
       <c r="C16" s="1"/>
@@ -849,8 +912,10 @@
       <c r="F16" s="1"/>
       <c r="G16" s="1"/>
       <c r="H16" s="1"/>
-    </row>
-    <row r="17" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I16" s="1"/>
+      <c r="J16" s="1"/>
+    </row>
+    <row r="17" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A17" s="1"/>
       <c r="B17" s="1"/>
       <c r="C17" s="1"/>
@@ -859,8 +924,10 @@
       <c r="F17" s="1"/>
       <c r="G17" s="1"/>
       <c r="H17" s="1"/>
-    </row>
-    <row r="18" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I17" s="1"/>
+      <c r="J17" s="1"/>
+    </row>
+    <row r="18" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A18" s="1"/>
       <c r="B18" s="1"/>
       <c r="C18" s="1"/>
@@ -869,8 +936,10 @@
       <c r="F18" s="1"/>
       <c r="G18" s="1"/>
       <c r="H18" s="1"/>
-    </row>
-    <row r="19" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I18" s="1"/>
+      <c r="J18" s="1"/>
+    </row>
+    <row r="19" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A19" s="1"/>
       <c r="B19" s="1"/>
       <c r="C19" s="1"/>
@@ -879,8 +948,10 @@
       <c r="F19" s="1"/>
       <c r="G19" s="1"/>
       <c r="H19" s="1"/>
-    </row>
-    <row r="20" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I19" s="1"/>
+      <c r="J19" s="1"/>
+    </row>
+    <row r="20" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A20" s="1"/>
       <c r="B20" s="1"/>
       <c r="C20" s="1"/>
@@ -889,8 +960,10 @@
       <c r="F20" s="1"/>
       <c r="G20" s="1"/>
       <c r="H20" s="1"/>
-    </row>
-    <row r="21" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I20" s="1"/>
+      <c r="J20" s="1"/>
+    </row>
+    <row r="21" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A21" s="1"/>
       <c r="B21" s="1"/>
       <c r="C21" s="1"/>
@@ -899,8 +972,10 @@
       <c r="F21" s="1"/>
       <c r="G21" s="1"/>
       <c r="H21" s="1"/>
-    </row>
-    <row r="22" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I21" s="1"/>
+      <c r="J21" s="1"/>
+    </row>
+    <row r="22" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A22" s="1"/>
       <c r="B22" s="1"/>
       <c r="C22" s="1"/>
@@ -909,8 +984,10 @@
       <c r="F22" s="1"/>
       <c r="G22" s="1"/>
       <c r="H22" s="1"/>
-    </row>
-    <row r="23" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I22" s="1"/>
+      <c r="J22" s="1"/>
+    </row>
+    <row r="23" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A23" s="1"/>
       <c r="B23" s="1"/>
       <c r="C23" s="1"/>
@@ -919,8 +996,10 @@
       <c r="F23" s="1"/>
       <c r="G23" s="1"/>
       <c r="H23" s="1"/>
-    </row>
-    <row r="24" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I23" s="1"/>
+      <c r="J23" s="1"/>
+    </row>
+    <row r="24" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A24" s="1"/>
       <c r="B24" s="1"/>
       <c r="C24" s="1"/>
@@ -929,8 +1008,10 @@
       <c r="F24" s="1"/>
       <c r="G24" s="1"/>
       <c r="H24" s="1"/>
-    </row>
-    <row r="25" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I24" s="1"/>
+      <c r="J24" s="1"/>
+    </row>
+    <row r="25" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A25" s="1"/>
       <c r="B25" s="1"/>
       <c r="C25" s="1"/>
@@ -939,8 +1020,10 @@
       <c r="F25" s="1"/>
       <c r="G25" s="1"/>
       <c r="H25" s="1"/>
-    </row>
-    <row r="26" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I25" s="1"/>
+      <c r="J25" s="1"/>
+    </row>
+    <row r="26" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A26" s="1"/>
       <c r="B26" s="1"/>
       <c r="C26" s="1"/>
@@ -949,8 +1032,10 @@
       <c r="F26" s="1"/>
       <c r="G26" s="1"/>
       <c r="H26" s="1"/>
-    </row>
-    <row r="27" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I26" s="1"/>
+      <c r="J26" s="1"/>
+    </row>
+    <row r="27" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A27" s="1"/>
       <c r="B27" s="1"/>
       <c r="C27" s="1"/>
@@ -959,8 +1044,10 @@
       <c r="F27" s="1"/>
       <c r="G27" s="1"/>
       <c r="H27" s="1"/>
-    </row>
-    <row r="28" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I27" s="1"/>
+      <c r="J27" s="1"/>
+    </row>
+    <row r="28" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A28" s="1"/>
       <c r="B28" s="1"/>
       <c r="C28" s="1"/>
@@ -969,8 +1056,10 @@
       <c r="F28" s="1"/>
       <c r="G28" s="1"/>
       <c r="H28" s="1"/>
-    </row>
-    <row r="29" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I28" s="1"/>
+      <c r="J28" s="1"/>
+    </row>
+    <row r="29" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A29" s="1"/>
       <c r="B29" s="1"/>
       <c r="C29" s="1"/>
@@ -979,8 +1068,10 @@
       <c r="F29" s="1"/>
       <c r="G29" s="1"/>
       <c r="H29" s="1"/>
-    </row>
-    <row r="30" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I29" s="1"/>
+      <c r="J29" s="1"/>
+    </row>
+    <row r="30" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A30" s="1"/>
       <c r="B30" s="1"/>
       <c r="C30" s="1"/>
@@ -989,8 +1080,10 @@
       <c r="F30" s="1"/>
       <c r="G30" s="1"/>
       <c r="H30" s="1"/>
-    </row>
-    <row r="31" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I30" s="1"/>
+      <c r="J30" s="1"/>
+    </row>
+    <row r="31" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A31" s="1"/>
       <c r="B31" s="1"/>
       <c r="C31" s="1"/>
@@ -999,8 +1092,10 @@
       <c r="F31" s="1"/>
       <c r="G31" s="1"/>
       <c r="H31" s="1"/>
-    </row>
-    <row r="32" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I31" s="1"/>
+      <c r="J31" s="1"/>
+    </row>
+    <row r="32" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A32" s="1"/>
       <c r="B32" s="1"/>
       <c r="C32" s="1"/>
@@ -1009,8 +1104,10 @@
       <c r="F32" s="1"/>
       <c r="G32" s="1"/>
       <c r="H32" s="1"/>
-    </row>
-    <row r="33" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I32" s="1"/>
+      <c r="J32" s="1"/>
+    </row>
+    <row r="33" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A33" s="1"/>
       <c r="B33" s="1"/>
       <c r="C33" s="1"/>
@@ -1019,8 +1116,10 @@
       <c r="F33" s="1"/>
       <c r="G33" s="1"/>
       <c r="H33" s="1"/>
-    </row>
-    <row r="34" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I33" s="1"/>
+      <c r="J33" s="1"/>
+    </row>
+    <row r="34" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A34" s="1"/>
       <c r="B34" s="1"/>
       <c r="C34" s="1"/>
@@ -1029,8 +1128,10 @@
       <c r="F34" s="1"/>
       <c r="G34" s="1"/>
       <c r="H34" s="1"/>
-    </row>
-    <row r="35" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I34" s="1"/>
+      <c r="J34" s="1"/>
+    </row>
+    <row r="35" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A35" s="1"/>
       <c r="B35" s="1"/>
       <c r="C35" s="1"/>
@@ -1039,8 +1140,10 @@
       <c r="F35" s="1"/>
       <c r="G35" s="1"/>
       <c r="H35" s="1"/>
-    </row>
-    <row r="36" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I35" s="1"/>
+      <c r="J35" s="1"/>
+    </row>
+    <row r="36" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A36" s="1"/>
       <c r="B36" s="1"/>
       <c r="C36" s="1"/>
@@ -1049,8 +1152,10 @@
       <c r="F36" s="1"/>
       <c r="G36" s="1"/>
       <c r="H36" s="1"/>
-    </row>
-    <row r="37" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I36" s="1"/>
+      <c r="J36" s="1"/>
+    </row>
+    <row r="37" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A37" s="1"/>
       <c r="B37" s="1"/>
       <c r="C37" s="1"/>
@@ -1059,8 +1164,10 @@
       <c r="F37" s="1"/>
       <c r="G37" s="1"/>
       <c r="H37" s="1"/>
-    </row>
-    <row r="38" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I37" s="1"/>
+      <c r="J37" s="1"/>
+    </row>
+    <row r="38" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A38" s="1"/>
       <c r="B38" s="1"/>
       <c r="C38" s="1"/>
@@ -1069,8 +1176,10 @@
       <c r="F38" s="1"/>
       <c r="G38" s="1"/>
       <c r="H38" s="1"/>
-    </row>
-    <row r="39" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I38" s="1"/>
+      <c r="J38" s="1"/>
+    </row>
+    <row r="39" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A39" s="1"/>
       <c r="B39" s="1"/>
       <c r="C39" s="1"/>
@@ -1079,8 +1188,10 @@
       <c r="F39" s="1"/>
       <c r="G39" s="1"/>
       <c r="H39" s="1"/>
-    </row>
-    <row r="40" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I39" s="1"/>
+      <c r="J39" s="1"/>
+    </row>
+    <row r="40" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A40" s="1"/>
       <c r="B40" s="1"/>
       <c r="C40" s="1"/>
@@ -1089,8 +1200,10 @@
       <c r="F40" s="1"/>
       <c r="G40" s="1"/>
       <c r="H40" s="1"/>
-    </row>
-    <row r="41" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I40" s="1"/>
+      <c r="J40" s="1"/>
+    </row>
+    <row r="41" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A41" s="1"/>
       <c r="B41" s="1"/>
       <c r="C41" s="1"/>
@@ -1099,8 +1212,10 @@
       <c r="F41" s="1"/>
       <c r="G41" s="1"/>
       <c r="H41" s="1"/>
-    </row>
-    <row r="42" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I41" s="1"/>
+      <c r="J41" s="1"/>
+    </row>
+    <row r="42" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A42" s="1"/>
       <c r="B42" s="1"/>
       <c r="C42" s="1"/>
@@ -1109,8 +1224,10 @@
       <c r="F42" s="1"/>
       <c r="G42" s="1"/>
       <c r="H42" s="1"/>
-    </row>
-    <row r="43" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I42" s="1"/>
+      <c r="J42" s="1"/>
+    </row>
+    <row r="43" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A43" s="1"/>
       <c r="B43" s="1"/>
       <c r="C43" s="1"/>
@@ -1119,8 +1236,10 @@
       <c r="F43" s="1"/>
       <c r="G43" s="1"/>
       <c r="H43" s="1"/>
-    </row>
-    <row r="44" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I43" s="1"/>
+      <c r="J43" s="1"/>
+    </row>
+    <row r="44" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A44" s="1"/>
       <c r="B44" s="1"/>
       <c r="C44" s="1"/>
@@ -1129,8 +1248,10 @@
       <c r="F44" s="1"/>
       <c r="G44" s="1"/>
       <c r="H44" s="1"/>
-    </row>
-    <row r="45" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I44" s="1"/>
+      <c r="J44" s="1"/>
+    </row>
+    <row r="45" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A45" s="1"/>
       <c r="B45" s="1"/>
       <c r="C45" s="1"/>
@@ -1139,8 +1260,10 @@
       <c r="F45" s="1"/>
       <c r="G45" s="1"/>
       <c r="H45" s="1"/>
-    </row>
-    <row r="46" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I45" s="1"/>
+      <c r="J45" s="1"/>
+    </row>
+    <row r="46" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A46" s="1"/>
       <c r="B46" s="1"/>
       <c r="C46" s="1"/>
@@ -1149,8 +1272,10 @@
       <c r="F46" s="1"/>
       <c r="G46" s="1"/>
       <c r="H46" s="1"/>
-    </row>
-    <row r="47" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I46" s="1"/>
+      <c r="J46" s="1"/>
+    </row>
+    <row r="47" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A47" s="1"/>
       <c r="B47" s="1"/>
       <c r="C47" s="1"/>
@@ -1159,12 +1284,24 @@
       <c r="F47" s="1"/>
       <c r="G47" s="1"/>
       <c r="H47" s="1"/>
+      <c r="I47" s="1"/>
+      <c r="J47" s="1"/>
     </row>
   </sheetData>
-  <mergeCells count="1">
-    <mergeCell ref="B1:E2"/>
+  <mergeCells count="11">
+    <mergeCell ref="B1:G2"/>
+    <mergeCell ref="C5:D5"/>
+    <mergeCell ref="C6:D6"/>
+    <mergeCell ref="C7:D7"/>
+    <mergeCell ref="C8:D8"/>
+    <mergeCell ref="F5:G5"/>
+    <mergeCell ref="F6:G6"/>
+    <mergeCell ref="F7:G7"/>
+    <mergeCell ref="F8:G8"/>
+    <mergeCell ref="C3:D3"/>
+    <mergeCell ref="F3:G3"/>
   </mergeCells>
-  <dataValidations count="1">
+  <dataValidations disablePrompts="1" count="1">
     <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Ebben a cellában a cég nevét, az alatta levőben a jelmondatát adhatja meg." sqref="B5" xr:uid="{63C8BD5B-0FB1-4721-BD42-C2B4B19CE83A}"/>
   </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
DMB10 - added unit tests and made minor changes to ui and generated excel
</commit_message>
<xml_diff>
--- a/DoMyBilling/DoMyBilling/ExcelBills/BillTemplate.xlsx
+++ b/DoMyBilling/DoMyBilling/ExcelBills/BillTemplate.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Kaposvári Márk\source\repos\IRF_Project\DoMyBilling\DoMyBilling\ExcelBills\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F025A0A0-A5A4-4BBE-80DB-FC09C0DB29E8}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D0AE73AA-1238-41DD-9A73-413FF5BFB35A}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{F2786273-DC1B-47B2-AC3A-962882F38129}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{F2786273-DC1B-47B2-AC3A-962882F38129}"/>
   </bookViews>
   <sheets>
     <sheet name="Munka1" sheetId="1" r:id="rId1"/>
@@ -62,9 +62,6 @@
     <t>Nettó egységár</t>
   </si>
   <si>
-    <t>Irányítószám, település:</t>
-  </si>
-  <si>
     <t>Utca és házszám:</t>
   </si>
   <si>
@@ -81,6 +78,9 @@
   </si>
   <si>
     <t>Áfa értéke</t>
+  </si>
+  <si>
+    <t>Ir.szám, település:</t>
   </si>
 </sst>
 </file>
@@ -296,9 +296,6 @@
     <xf numFmtId="0" fontId="0" fillId="3" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -352,6 +349,15 @@
     </xf>
     <xf numFmtId="0" fontId="3" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -668,146 +674,138 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6DEC2F63-A0AF-4687-BE6D-74EE77351709}">
-  <dimension ref="A1:J47"/>
+  <dimension ref="A1:I47"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E11" sqref="E11"/>
+      <selection activeCell="A4" sqref="A4:C4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="22" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="16.42578125" customWidth="1"/>
-    <col min="4" max="4" width="21" customWidth="1"/>
-    <col min="5" max="5" width="23.140625" customWidth="1"/>
-    <col min="6" max="6" width="22" customWidth="1"/>
-    <col min="7" max="7" width="18.42578125" customWidth="1"/>
-    <col min="8" max="8" width="9.140625" customWidth="1"/>
+    <col min="1" max="1" width="20" customWidth="1"/>
+    <col min="2" max="2" width="16.42578125" customWidth="1"/>
+    <col min="3" max="3" width="10.28515625" customWidth="1"/>
+    <col min="4" max="4" width="19.5703125" customWidth="1"/>
+    <col min="5" max="5" width="17.140625" customWidth="1"/>
+    <col min="6" max="6" width="13.85546875" customWidth="1"/>
+    <col min="7" max="7" width="9.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A1" s="1"/>
-      <c r="B1" s="11" t="s">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A1" s="8" t="s">
         <v>5</v>
       </c>
-      <c r="C1" s="12"/>
-      <c r="D1" s="12"/>
-      <c r="E1" s="12"/>
-      <c r="F1" s="12"/>
-      <c r="G1" s="13"/>
+      <c r="B1" s="9"/>
+      <c r="C1" s="9"/>
+      <c r="D1" s="9"/>
+      <c r="E1" s="9"/>
+      <c r="F1" s="10"/>
+      <c r="G1" s="1"/>
       <c r="H1" s="1"/>
       <c r="I1" s="1"/>
-      <c r="J1" s="1"/>
-    </row>
-    <row r="2" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="1"/>
-      <c r="B2" s="14"/>
-      <c r="C2" s="15"/>
-      <c r="D2" s="15"/>
-      <c r="E2" s="15"/>
-      <c r="F2" s="15"/>
-      <c r="G2" s="16"/>
+    </row>
+    <row r="2" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A2" s="11"/>
+      <c r="B2" s="12"/>
+      <c r="C2" s="12"/>
+      <c r="D2" s="12"/>
+      <c r="E2" s="12"/>
+      <c r="F2" s="13"/>
+      <c r="G2" s="1"/>
       <c r="H2" s="1"/>
       <c r="I2" s="1"/>
-      <c r="J2" s="1"/>
-    </row>
-    <row r="3" spans="1:10" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="1"/>
-      <c r="B3" s="17" t="s">
-        <v>13</v>
-      </c>
-      <c r="C3" s="27"/>
-      <c r="D3" s="27"/>
-      <c r="E3" s="18" t="s">
+    </row>
+    <row r="3" spans="1:9" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A3" s="14" t="s">
         <v>12</v>
       </c>
-      <c r="F3" s="27"/>
-      <c r="G3" s="28"/>
+      <c r="B3" s="24"/>
+      <c r="C3" s="24"/>
+      <c r="D3" s="15" t="s">
+        <v>11</v>
+      </c>
+      <c r="E3" s="24"/>
+      <c r="F3" s="25"/>
+      <c r="G3" s="1"/>
       <c r="H3" s="1"/>
       <c r="I3" s="1"/>
-      <c r="J3" s="1"/>
-    </row>
-    <row r="4" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="1"/>
-      <c r="B4" s="8" t="s">
+    </row>
+    <row r="4" spans="1:9" ht="22.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A4" s="26" t="s">
         <v>1</v>
       </c>
-      <c r="C4" s="9"/>
-      <c r="D4" s="9"/>
-      <c r="E4" s="9" t="s">
+      <c r="B4" s="27"/>
+      <c r="C4" s="27"/>
+      <c r="D4" s="27" t="s">
         <v>3</v>
       </c>
-      <c r="F4" s="9"/>
-      <c r="G4" s="10"/>
+      <c r="E4" s="27"/>
+      <c r="F4" s="28"/>
+      <c r="G4" s="1"/>
       <c r="H4" s="1"/>
       <c r="I4" s="1"/>
-      <c r="J4" s="1"/>
-    </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A5" s="1"/>
-      <c r="B5" s="2" t="s">
+    </row>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A5" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="C5" s="19"/>
-      <c r="D5" s="20"/>
-      <c r="E5" s="2" t="s">
+      <c r="B5" s="16"/>
+      <c r="C5" s="17"/>
+      <c r="D5" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="F5" s="19"/>
-      <c r="G5" s="20"/>
+      <c r="E5" s="16"/>
+      <c r="F5" s="17"/>
+      <c r="G5" s="1"/>
       <c r="H5" s="1"/>
       <c r="I5" s="1"/>
-      <c r="J5" s="1"/>
-    </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A6" s="1"/>
-      <c r="B6" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="C6" s="21"/>
-      <c r="D6" s="22"/>
-      <c r="E6" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="F6" s="21"/>
-      <c r="G6" s="22"/>
+    </row>
+    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A6" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="B6" s="18"/>
+      <c r="C6" s="19"/>
+      <c r="D6" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="E6" s="18"/>
+      <c r="F6" s="19"/>
+      <c r="G6" s="1"/>
       <c r="H6" s="1"/>
       <c r="I6" s="1"/>
-      <c r="J6" s="1"/>
-    </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A7" s="1"/>
-      <c r="B7" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="C7" s="21"/>
-      <c r="D7" s="22"/>
-      <c r="E7" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="F7" s="21"/>
-      <c r="G7" s="22"/>
+    </row>
+    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A7" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="B7" s="18"/>
+      <c r="C7" s="19"/>
+      <c r="D7" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="E7" s="18"/>
+      <c r="F7" s="19"/>
+      <c r="G7" s="1"/>
       <c r="H7" s="1"/>
       <c r="I7" s="1"/>
-      <c r="J7" s="1"/>
-    </row>
-    <row r="8" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A8" s="1"/>
-      <c r="B8" s="4" t="s">
+    </row>
+    <row r="8" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A8" s="4" t="s">
         <v>0</v>
       </c>
-      <c r="C8" s="23"/>
-      <c r="D8" s="24"/>
-      <c r="E8" s="4" t="s">
+      <c r="B8" s="20"/>
+      <c r="C8" s="21"/>
+      <c r="D8" s="4" t="s">
         <v>0</v>
       </c>
-      <c r="F8" s="25"/>
-      <c r="G8" s="26"/>
+      <c r="E8" s="22"/>
+      <c r="F8" s="23"/>
+      <c r="G8" s="1"/>
       <c r="H8" s="1"/>
       <c r="I8" s="1"/>
-      <c r="J8" s="1"/>
-    </row>
-    <row r="9" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    </row>
+    <row r="9" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A9" s="1"/>
       <c r="B9" s="1"/>
       <c r="C9" s="1"/>
@@ -817,15 +815,16 @@
       <c r="G9" s="1"/>
       <c r="H9" s="1"/>
       <c r="I9" s="1"/>
-      <c r="J9" s="1"/>
-    </row>
-    <row r="10" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A10" s="1"/>
-      <c r="B10" s="5" t="s">
+    </row>
+    <row r="10" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A10" s="5" t="s">
         <v>6</v>
       </c>
+      <c r="B10" s="6" t="s">
+        <v>7</v>
+      </c>
       <c r="C10" s="6" t="s">
-        <v>7</v>
+        <v>13</v>
       </c>
       <c r="D10" s="6" t="s">
         <v>8</v>
@@ -833,17 +832,14 @@
       <c r="E10" s="6" t="s">
         <v>14</v>
       </c>
-      <c r="F10" s="6" t="s">
-        <v>15</v>
-      </c>
-      <c r="G10" s="7" t="s">
-        <v>11</v>
-      </c>
+      <c r="F10" s="7" t="s">
+        <v>10</v>
+      </c>
+      <c r="G10" s="1"/>
       <c r="H10" s="1"/>
       <c r="I10" s="1"/>
-      <c r="J10" s="1"/>
-    </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
+    </row>
+    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A11" s="1"/>
       <c r="B11" s="1"/>
       <c r="C11" s="1"/>
@@ -853,9 +849,8 @@
       <c r="G11" s="1"/>
       <c r="H11" s="1"/>
       <c r="I11" s="1"/>
-      <c r="J11" s="1"/>
-    </row>
-    <row r="12" spans="1:10" x14ac:dyDescent="0.25">
+    </row>
+    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A12" s="1"/>
       <c r="B12" s="1"/>
       <c r="C12" s="1"/>
@@ -865,9 +860,8 @@
       <c r="G12" s="1"/>
       <c r="H12" s="1"/>
       <c r="I12" s="1"/>
-      <c r="J12" s="1"/>
-    </row>
-    <row r="13" spans="1:10" x14ac:dyDescent="0.25">
+    </row>
+    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A13" s="1"/>
       <c r="B13" s="1"/>
       <c r="C13" s="1"/>
@@ -877,9 +871,8 @@
       <c r="G13" s="1"/>
       <c r="H13" s="1"/>
       <c r="I13" s="1"/>
-      <c r="J13" s="1"/>
-    </row>
-    <row r="14" spans="1:10" x14ac:dyDescent="0.25">
+    </row>
+    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A14" s="1"/>
       <c r="B14" s="1"/>
       <c r="C14" s="1"/>
@@ -889,9 +882,8 @@
       <c r="G14" s="1"/>
       <c r="H14" s="1"/>
       <c r="I14" s="1"/>
-      <c r="J14" s="1"/>
-    </row>
-    <row r="15" spans="1:10" x14ac:dyDescent="0.25">
+    </row>
+    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A15" s="1"/>
       <c r="B15" s="1"/>
       <c r="C15" s="1"/>
@@ -901,9 +893,8 @@
       <c r="G15" s="1"/>
       <c r="H15" s="1"/>
       <c r="I15" s="1"/>
-      <c r="J15" s="1"/>
-    </row>
-    <row r="16" spans="1:10" x14ac:dyDescent="0.25">
+    </row>
+    <row r="16" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A16" s="1"/>
       <c r="B16" s="1"/>
       <c r="C16" s="1"/>
@@ -913,9 +904,8 @@
       <c r="G16" s="1"/>
       <c r="H16" s="1"/>
       <c r="I16" s="1"/>
-      <c r="J16" s="1"/>
-    </row>
-    <row r="17" spans="1:10" x14ac:dyDescent="0.25">
+    </row>
+    <row r="17" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A17" s="1"/>
       <c r="B17" s="1"/>
       <c r="C17" s="1"/>
@@ -925,9 +915,8 @@
       <c r="G17" s="1"/>
       <c r="H17" s="1"/>
       <c r="I17" s="1"/>
-      <c r="J17" s="1"/>
-    </row>
-    <row r="18" spans="1:10" x14ac:dyDescent="0.25">
+    </row>
+    <row r="18" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A18" s="1"/>
       <c r="B18" s="1"/>
       <c r="C18" s="1"/>
@@ -937,9 +926,8 @@
       <c r="G18" s="1"/>
       <c r="H18" s="1"/>
       <c r="I18" s="1"/>
-      <c r="J18" s="1"/>
-    </row>
-    <row r="19" spans="1:10" x14ac:dyDescent="0.25">
+    </row>
+    <row r="19" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A19" s="1"/>
       <c r="B19" s="1"/>
       <c r="C19" s="1"/>
@@ -949,9 +937,8 @@
       <c r="G19" s="1"/>
       <c r="H19" s="1"/>
       <c r="I19" s="1"/>
-      <c r="J19" s="1"/>
-    </row>
-    <row r="20" spans="1:10" x14ac:dyDescent="0.25">
+    </row>
+    <row r="20" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A20" s="1"/>
       <c r="B20" s="1"/>
       <c r="C20" s="1"/>
@@ -961,9 +948,8 @@
       <c r="G20" s="1"/>
       <c r="H20" s="1"/>
       <c r="I20" s="1"/>
-      <c r="J20" s="1"/>
-    </row>
-    <row r="21" spans="1:10" x14ac:dyDescent="0.25">
+    </row>
+    <row r="21" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A21" s="1"/>
       <c r="B21" s="1"/>
       <c r="C21" s="1"/>
@@ -973,9 +959,8 @@
       <c r="G21" s="1"/>
       <c r="H21" s="1"/>
       <c r="I21" s="1"/>
-      <c r="J21" s="1"/>
-    </row>
-    <row r="22" spans="1:10" x14ac:dyDescent="0.25">
+    </row>
+    <row r="22" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A22" s="1"/>
       <c r="B22" s="1"/>
       <c r="C22" s="1"/>
@@ -985,9 +970,8 @@
       <c r="G22" s="1"/>
       <c r="H22" s="1"/>
       <c r="I22" s="1"/>
-      <c r="J22" s="1"/>
-    </row>
-    <row r="23" spans="1:10" x14ac:dyDescent="0.25">
+    </row>
+    <row r="23" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A23" s="1"/>
       <c r="B23" s="1"/>
       <c r="C23" s="1"/>
@@ -997,9 +981,8 @@
       <c r="G23" s="1"/>
       <c r="H23" s="1"/>
       <c r="I23" s="1"/>
-      <c r="J23" s="1"/>
-    </row>
-    <row r="24" spans="1:10" x14ac:dyDescent="0.25">
+    </row>
+    <row r="24" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A24" s="1"/>
       <c r="B24" s="1"/>
       <c r="C24" s="1"/>
@@ -1009,9 +992,8 @@
       <c r="G24" s="1"/>
       <c r="H24" s="1"/>
       <c r="I24" s="1"/>
-      <c r="J24" s="1"/>
-    </row>
-    <row r="25" spans="1:10" x14ac:dyDescent="0.25">
+    </row>
+    <row r="25" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A25" s="1"/>
       <c r="B25" s="1"/>
       <c r="C25" s="1"/>
@@ -1021,9 +1003,8 @@
       <c r="G25" s="1"/>
       <c r="H25" s="1"/>
       <c r="I25" s="1"/>
-      <c r="J25" s="1"/>
-    </row>
-    <row r="26" spans="1:10" x14ac:dyDescent="0.25">
+    </row>
+    <row r="26" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A26" s="1"/>
       <c r="B26" s="1"/>
       <c r="C26" s="1"/>
@@ -1033,9 +1014,8 @@
       <c r="G26" s="1"/>
       <c r="H26" s="1"/>
       <c r="I26" s="1"/>
-      <c r="J26" s="1"/>
-    </row>
-    <row r="27" spans="1:10" x14ac:dyDescent="0.25">
+    </row>
+    <row r="27" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A27" s="1"/>
       <c r="B27" s="1"/>
       <c r="C27" s="1"/>
@@ -1045,9 +1025,8 @@
       <c r="G27" s="1"/>
       <c r="H27" s="1"/>
       <c r="I27" s="1"/>
-      <c r="J27" s="1"/>
-    </row>
-    <row r="28" spans="1:10" x14ac:dyDescent="0.25">
+    </row>
+    <row r="28" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A28" s="1"/>
       <c r="B28" s="1"/>
       <c r="C28" s="1"/>
@@ -1057,9 +1036,8 @@
       <c r="G28" s="1"/>
       <c r="H28" s="1"/>
       <c r="I28" s="1"/>
-      <c r="J28" s="1"/>
-    </row>
-    <row r="29" spans="1:10" x14ac:dyDescent="0.25">
+    </row>
+    <row r="29" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A29" s="1"/>
       <c r="B29" s="1"/>
       <c r="C29" s="1"/>
@@ -1069,9 +1047,8 @@
       <c r="G29" s="1"/>
       <c r="H29" s="1"/>
       <c r="I29" s="1"/>
-      <c r="J29" s="1"/>
-    </row>
-    <row r="30" spans="1:10" x14ac:dyDescent="0.25">
+    </row>
+    <row r="30" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A30" s="1"/>
       <c r="B30" s="1"/>
       <c r="C30" s="1"/>
@@ -1081,9 +1058,8 @@
       <c r="G30" s="1"/>
       <c r="H30" s="1"/>
       <c r="I30" s="1"/>
-      <c r="J30" s="1"/>
-    </row>
-    <row r="31" spans="1:10" x14ac:dyDescent="0.25">
+    </row>
+    <row r="31" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A31" s="1"/>
       <c r="B31" s="1"/>
       <c r="C31" s="1"/>
@@ -1093,9 +1069,8 @@
       <c r="G31" s="1"/>
       <c r="H31" s="1"/>
       <c r="I31" s="1"/>
-      <c r="J31" s="1"/>
-    </row>
-    <row r="32" spans="1:10" x14ac:dyDescent="0.25">
+    </row>
+    <row r="32" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A32" s="1"/>
       <c r="B32" s="1"/>
       <c r="C32" s="1"/>
@@ -1105,9 +1080,8 @@
       <c r="G32" s="1"/>
       <c r="H32" s="1"/>
       <c r="I32" s="1"/>
-      <c r="J32" s="1"/>
-    </row>
-    <row r="33" spans="1:10" x14ac:dyDescent="0.25">
+    </row>
+    <row r="33" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A33" s="1"/>
       <c r="B33" s="1"/>
       <c r="C33" s="1"/>
@@ -1117,9 +1091,8 @@
       <c r="G33" s="1"/>
       <c r="H33" s="1"/>
       <c r="I33" s="1"/>
-      <c r="J33" s="1"/>
-    </row>
-    <row r="34" spans="1:10" x14ac:dyDescent="0.25">
+    </row>
+    <row r="34" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A34" s="1"/>
       <c r="B34" s="1"/>
       <c r="C34" s="1"/>
@@ -1129,9 +1102,8 @@
       <c r="G34" s="1"/>
       <c r="H34" s="1"/>
       <c r="I34" s="1"/>
-      <c r="J34" s="1"/>
-    </row>
-    <row r="35" spans="1:10" x14ac:dyDescent="0.25">
+    </row>
+    <row r="35" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A35" s="1"/>
       <c r="B35" s="1"/>
       <c r="C35" s="1"/>
@@ -1141,9 +1113,8 @@
       <c r="G35" s="1"/>
       <c r="H35" s="1"/>
       <c r="I35" s="1"/>
-      <c r="J35" s="1"/>
-    </row>
-    <row r="36" spans="1:10" x14ac:dyDescent="0.25">
+    </row>
+    <row r="36" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A36" s="1"/>
       <c r="B36" s="1"/>
       <c r="C36" s="1"/>
@@ -1153,9 +1124,8 @@
       <c r="G36" s="1"/>
       <c r="H36" s="1"/>
       <c r="I36" s="1"/>
-      <c r="J36" s="1"/>
-    </row>
-    <row r="37" spans="1:10" x14ac:dyDescent="0.25">
+    </row>
+    <row r="37" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A37" s="1"/>
       <c r="B37" s="1"/>
       <c r="C37" s="1"/>
@@ -1165,9 +1135,8 @@
       <c r="G37" s="1"/>
       <c r="H37" s="1"/>
       <c r="I37" s="1"/>
-      <c r="J37" s="1"/>
-    </row>
-    <row r="38" spans="1:10" x14ac:dyDescent="0.25">
+    </row>
+    <row r="38" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A38" s="1"/>
       <c r="B38" s="1"/>
       <c r="C38" s="1"/>
@@ -1177,9 +1146,8 @@
       <c r="G38" s="1"/>
       <c r="H38" s="1"/>
       <c r="I38" s="1"/>
-      <c r="J38" s="1"/>
-    </row>
-    <row r="39" spans="1:10" x14ac:dyDescent="0.25">
+    </row>
+    <row r="39" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A39" s="1"/>
       <c r="B39" s="1"/>
       <c r="C39" s="1"/>
@@ -1189,9 +1157,8 @@
       <c r="G39" s="1"/>
       <c r="H39" s="1"/>
       <c r="I39" s="1"/>
-      <c r="J39" s="1"/>
-    </row>
-    <row r="40" spans="1:10" x14ac:dyDescent="0.25">
+    </row>
+    <row r="40" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A40" s="1"/>
       <c r="B40" s="1"/>
       <c r="C40" s="1"/>
@@ -1201,9 +1168,8 @@
       <c r="G40" s="1"/>
       <c r="H40" s="1"/>
       <c r="I40" s="1"/>
-      <c r="J40" s="1"/>
-    </row>
-    <row r="41" spans="1:10" x14ac:dyDescent="0.25">
+    </row>
+    <row r="41" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A41" s="1"/>
       <c r="B41" s="1"/>
       <c r="C41" s="1"/>
@@ -1213,9 +1179,8 @@
       <c r="G41" s="1"/>
       <c r="H41" s="1"/>
       <c r="I41" s="1"/>
-      <c r="J41" s="1"/>
-    </row>
-    <row r="42" spans="1:10" x14ac:dyDescent="0.25">
+    </row>
+    <row r="42" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A42" s="1"/>
       <c r="B42" s="1"/>
       <c r="C42" s="1"/>
@@ -1225,9 +1190,8 @@
       <c r="G42" s="1"/>
       <c r="H42" s="1"/>
       <c r="I42" s="1"/>
-      <c r="J42" s="1"/>
-    </row>
-    <row r="43" spans="1:10" x14ac:dyDescent="0.25">
+    </row>
+    <row r="43" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A43" s="1"/>
       <c r="B43" s="1"/>
       <c r="C43" s="1"/>
@@ -1237,9 +1201,8 @@
       <c r="G43" s="1"/>
       <c r="H43" s="1"/>
       <c r="I43" s="1"/>
-      <c r="J43" s="1"/>
-    </row>
-    <row r="44" spans="1:10" x14ac:dyDescent="0.25">
+    </row>
+    <row r="44" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A44" s="1"/>
       <c r="B44" s="1"/>
       <c r="C44" s="1"/>
@@ -1249,9 +1212,8 @@
       <c r="G44" s="1"/>
       <c r="H44" s="1"/>
       <c r="I44" s="1"/>
-      <c r="J44" s="1"/>
-    </row>
-    <row r="45" spans="1:10" x14ac:dyDescent="0.25">
+    </row>
+    <row r="45" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A45" s="1"/>
       <c r="B45" s="1"/>
       <c r="C45" s="1"/>
@@ -1261,9 +1223,8 @@
       <c r="G45" s="1"/>
       <c r="H45" s="1"/>
       <c r="I45" s="1"/>
-      <c r="J45" s="1"/>
-    </row>
-    <row r="46" spans="1:10" x14ac:dyDescent="0.25">
+    </row>
+    <row r="46" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A46" s="1"/>
       <c r="B46" s="1"/>
       <c r="C46" s="1"/>
@@ -1273,9 +1234,8 @@
       <c r="G46" s="1"/>
       <c r="H46" s="1"/>
       <c r="I46" s="1"/>
-      <c r="J46" s="1"/>
-    </row>
-    <row r="47" spans="1:10" x14ac:dyDescent="0.25">
+    </row>
+    <row r="47" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A47" s="1"/>
       <c r="B47" s="1"/>
       <c r="C47" s="1"/>
@@ -1285,26 +1245,27 @@
       <c r="G47" s="1"/>
       <c r="H47" s="1"/>
       <c r="I47" s="1"/>
-      <c r="J47" s="1"/>
     </row>
   </sheetData>
-  <mergeCells count="11">
-    <mergeCell ref="B1:G2"/>
-    <mergeCell ref="C5:D5"/>
-    <mergeCell ref="C6:D6"/>
-    <mergeCell ref="C7:D7"/>
-    <mergeCell ref="C8:D8"/>
-    <mergeCell ref="F5:G5"/>
-    <mergeCell ref="F6:G6"/>
-    <mergeCell ref="F7:G7"/>
-    <mergeCell ref="F8:G8"/>
-    <mergeCell ref="C3:D3"/>
-    <mergeCell ref="F3:G3"/>
+  <mergeCells count="13">
+    <mergeCell ref="A1:F2"/>
+    <mergeCell ref="B5:C5"/>
+    <mergeCell ref="B6:C6"/>
+    <mergeCell ref="B7:C7"/>
+    <mergeCell ref="B8:C8"/>
+    <mergeCell ref="E5:F5"/>
+    <mergeCell ref="E6:F6"/>
+    <mergeCell ref="E7:F7"/>
+    <mergeCell ref="E8:F8"/>
+    <mergeCell ref="B3:C3"/>
+    <mergeCell ref="E3:F3"/>
+    <mergeCell ref="A4:C4"/>
+    <mergeCell ref="D4:F4"/>
   </mergeCells>
   <dataValidations disablePrompts="1" count="1">
-    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Ebben a cellában a cég nevét, az alatta levőben a jelmondatát adhatja meg." sqref="B5" xr:uid="{63C8BD5B-0FB1-4721-BD42-C2B4B19CE83A}"/>
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Ebben a cellában a cég nevét, az alatta levőben a jelmondatát adhatja meg." sqref="A5" xr:uid="{63C8BD5B-0FB1-4721-BD42-C2B4B19CE83A}"/>
   </dataValidations>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageMargins left="0.25" right="0.25" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
DMB11 - made further changes to the generated excel
</commit_message>
<xml_diff>
--- a/DoMyBilling/DoMyBilling/ExcelBills/BillTemplate.xlsx
+++ b/DoMyBilling/DoMyBilling/ExcelBills/BillTemplate.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Kaposvári Márk\source\repos\IRF_Project\DoMyBilling\DoMyBilling\ExcelBills\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D0AE73AA-1238-41DD-9A73-413FF5BFB35A}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B56D37CB-EA69-42D6-AFCB-39F1E4AD7A46}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{F2786273-DC1B-47B2-AC3A-962882F38129}"/>
   </bookViews>
@@ -677,7 +677,7 @@
   <dimension ref="A1:I47"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A4" sqref="A4:C4"/>
+      <selection activeCell="E5" sqref="E5:F5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>